<commit_message>
V100 : Initialisation du projet
</commit_message>
<xml_diff>
--- a/DisplayFont/doc/UWP Horloge - Version 100.xlsx
+++ b/DisplayFont/doc/UWP Horloge - Version 100.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E1B81C-4E8D-4230-95D3-0A81238E4549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A66B9BD-BA31-4985-8B8E-876C7EA946D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="665" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Page de garde" sheetId="17" r:id="rId1"/>
+    <sheet name="Raspberry Pi GPIO" sheetId="17" r:id="rId1"/>
     <sheet name="LCD 240x320 - Caractère 5x7" sheetId="1" r:id="rId2"/>
     <sheet name="Tableau des 256 caractères 5x7" sheetId="16" r:id="rId3"/>
     <sheet name="Tables de conversion" sheetId="5" r:id="rId4"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5142" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5182" uniqueCount="310">
   <si>
     <t>A</t>
   </si>
@@ -930,12 +930,36 @@
   <si>
     <t xml:space="preserve">7 </t>
   </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -988,8 +1012,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1023,6 +1061,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6666FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1363,7 +1443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1658,13 +1738,13 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1676,6 +1756,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1684,6 +1775,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CCFF"/>
+      <color rgb="FF6666FF"/>
+      <color rgb="FFFF3399"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF00FF00"/>
     </mruColors>
@@ -1962,9 +2056,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FC8846-D7E0-4274-ABFC-E077D17348CE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1973,10 +2067,211 @@
     <col min="1" max="16384" width="3.7109375" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39"/>
     </row>
+    <row r="11" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="106" t="s">
+        <v>70</v>
+      </c>
+      <c r="R11" s="107"/>
+      <c r="S11" s="112"/>
+      <c r="T11" s="106" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="R12" s="108"/>
+      <c r="S12" s="112"/>
+      <c r="T12" s="106" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q13" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="R13" s="108"/>
+      <c r="S13" s="110"/>
+      <c r="T13" s="106" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" s="109"/>
+      <c r="S14" s="113"/>
+      <c r="T14" s="106" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="106" t="s">
+        <v>85</v>
+      </c>
+      <c r="R15" s="110"/>
+      <c r="S15" s="113"/>
+      <c r="T15" s="106" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q16" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="R16" s="109"/>
+      <c r="S16" s="114"/>
+      <c r="T16" s="106" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" s="109"/>
+      <c r="S17" s="110"/>
+      <c r="T17" s="106" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q18" s="106" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" s="109"/>
+      <c r="S18" s="109"/>
+      <c r="T18" s="106" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="19" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q19" s="106" t="s">
+        <v>282</v>
+      </c>
+      <c r="R19" s="107"/>
+      <c r="S19" s="109"/>
+      <c r="T19" s="106" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="106" t="s">
+        <v>284</v>
+      </c>
+      <c r="R20" s="111"/>
+      <c r="S20" s="110"/>
+      <c r="T20" s="106" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="106" t="s">
+        <v>286</v>
+      </c>
+      <c r="R21" s="111"/>
+      <c r="S21" s="109"/>
+      <c r="T21" s="106" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q22" s="106" t="s">
+        <v>288</v>
+      </c>
+      <c r="R22" s="111"/>
+      <c r="S22" s="111"/>
+      <c r="T22" s="106" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q23" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="R23" s="110"/>
+      <c r="S23" s="111"/>
+      <c r="T23" s="106" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q24" s="106" t="s">
+        <v>295</v>
+      </c>
+      <c r="R24" s="108"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="106" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="25" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q25" s="106" t="s">
+        <v>297</v>
+      </c>
+      <c r="R25" s="109"/>
+      <c r="S25" s="110"/>
+      <c r="T25" s="106" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="26" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q26" s="106" t="s">
+        <v>299</v>
+      </c>
+      <c r="R26" s="109"/>
+      <c r="S26" s="109"/>
+      <c r="T26" s="106" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="27" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q27" s="106" t="s">
+        <v>302</v>
+      </c>
+      <c r="R27" s="109"/>
+      <c r="S27" s="110"/>
+      <c r="T27" s="106" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q28" s="106" t="s">
+        <v>303</v>
+      </c>
+      <c r="R28" s="114"/>
+      <c r="S28" s="109"/>
+      <c r="T28" s="106" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q29" s="106" t="s">
+        <v>304</v>
+      </c>
+      <c r="R29" s="109"/>
+      <c r="S29" s="114"/>
+      <c r="T29" s="106" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="30" spans="17:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q30" s="106" t="s">
+        <v>305</v>
+      </c>
+      <c r="R30" s="110"/>
+      <c r="S30" s="114"/>
+      <c r="T30" s="106" t="s">
+        <v>309</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2746,7 +3041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7B969B-1595-4B5D-B065-0D30FB5BFD17}">
   <dimension ref="A2:ADT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="UL1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="UL1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="XP48" sqref="XP48"/>
     </sheetView>
   </sheetViews>
@@ -43732,87 +44027,285 @@
     </row>
   </sheetData>
   <mergeCells count="384">
-    <mergeCell ref="C51:Q51"/>
-    <mergeCell ref="R51:S51"/>
-    <mergeCell ref="T51:U51"/>
-    <mergeCell ref="W51:X51"/>
-    <mergeCell ref="AC3:AD4"/>
-    <mergeCell ref="AC39:AD40"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="P3:Q4"/>
-    <mergeCell ref="D39:E40"/>
-    <mergeCell ref="P39:Q40"/>
-    <mergeCell ref="P27:Q28"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="P15:Q16"/>
-    <mergeCell ref="AO39:AP40"/>
-    <mergeCell ref="AB51:AP51"/>
-    <mergeCell ref="AQ51:AR51"/>
-    <mergeCell ref="AS51:AT51"/>
-    <mergeCell ref="AV51:AW51"/>
-    <mergeCell ref="AO3:AP4"/>
-    <mergeCell ref="AC15:AD16"/>
-    <mergeCell ref="AO15:AP16"/>
-    <mergeCell ref="AC27:AD28"/>
-    <mergeCell ref="AO27:AP28"/>
-    <mergeCell ref="BB39:BC40"/>
-    <mergeCell ref="BN39:BO40"/>
-    <mergeCell ref="BA51:BO51"/>
-    <mergeCell ref="BP51:BQ51"/>
-    <mergeCell ref="BR51:BS51"/>
-    <mergeCell ref="BB3:BC4"/>
-    <mergeCell ref="BN3:BO4"/>
-    <mergeCell ref="BB15:BC16"/>
-    <mergeCell ref="BN15:BO16"/>
-    <mergeCell ref="BB27:BC28"/>
-    <mergeCell ref="BN27:BO28"/>
-    <mergeCell ref="BU51:BV51"/>
-    <mergeCell ref="CA3:CB4"/>
-    <mergeCell ref="CM3:CN4"/>
-    <mergeCell ref="CA15:CB16"/>
-    <mergeCell ref="CM15:CN16"/>
-    <mergeCell ref="CA27:CB28"/>
-    <mergeCell ref="CM27:CN28"/>
-    <mergeCell ref="CA39:CB40"/>
-    <mergeCell ref="CM39:CN40"/>
-    <mergeCell ref="BZ51:CN51"/>
-    <mergeCell ref="CO51:CP51"/>
-    <mergeCell ref="CQ51:CR51"/>
-    <mergeCell ref="CT51:CU51"/>
-    <mergeCell ref="CZ3:DA4"/>
-    <mergeCell ref="DL3:DM4"/>
-    <mergeCell ref="CZ15:DA16"/>
-    <mergeCell ref="DL15:DM16"/>
-    <mergeCell ref="CZ27:DA28"/>
-    <mergeCell ref="DL27:DM28"/>
-    <mergeCell ref="CZ39:DA40"/>
-    <mergeCell ref="DL39:DM40"/>
-    <mergeCell ref="CY51:DM51"/>
-    <mergeCell ref="DN51:DO51"/>
-    <mergeCell ref="DP51:DQ51"/>
-    <mergeCell ref="DS51:DT51"/>
-    <mergeCell ref="DY3:DZ4"/>
-    <mergeCell ref="EK3:EL4"/>
-    <mergeCell ref="DY15:DZ16"/>
-    <mergeCell ref="EK15:EL16"/>
-    <mergeCell ref="DY27:DZ28"/>
-    <mergeCell ref="EK27:EL28"/>
-    <mergeCell ref="DY39:DZ40"/>
-    <mergeCell ref="EK39:EL40"/>
-    <mergeCell ref="DX51:EL51"/>
-    <mergeCell ref="EM51:EN51"/>
-    <mergeCell ref="EO51:EP51"/>
-    <mergeCell ref="ER51:ES51"/>
-    <mergeCell ref="EX3:EY4"/>
-    <mergeCell ref="FJ3:FK4"/>
-    <mergeCell ref="EX15:EY16"/>
-    <mergeCell ref="FJ15:FK16"/>
-    <mergeCell ref="EX27:EY28"/>
-    <mergeCell ref="FJ27:FK28"/>
-    <mergeCell ref="EX39:EY40"/>
-    <mergeCell ref="FJ39:FK40"/>
-    <mergeCell ref="EW51:FK51"/>
+    <mergeCell ref="ACX51:ADL51"/>
+    <mergeCell ref="ADM51:ADN51"/>
+    <mergeCell ref="ADO51:ADP51"/>
+    <mergeCell ref="ADR51:ADS51"/>
+    <mergeCell ref="ABT51:ABU51"/>
+    <mergeCell ref="ABY51:ACM51"/>
+    <mergeCell ref="ACN51:ACO51"/>
+    <mergeCell ref="ACP51:ACQ51"/>
+    <mergeCell ref="ACS51:ACT51"/>
+    <mergeCell ref="AAR51:AAS51"/>
+    <mergeCell ref="AAU51:AAV51"/>
+    <mergeCell ref="AAZ51:ABN51"/>
+    <mergeCell ref="ABO51:ABP51"/>
+    <mergeCell ref="ABQ51:ABR51"/>
+    <mergeCell ref="ZQ51:ZR51"/>
+    <mergeCell ref="ZS51:ZT51"/>
+    <mergeCell ref="ZV51:ZW51"/>
+    <mergeCell ref="AAA51:AAO51"/>
+    <mergeCell ref="AAP51:AAQ51"/>
+    <mergeCell ref="YC51:YQ51"/>
+    <mergeCell ref="YR51:YS51"/>
+    <mergeCell ref="YT51:YU51"/>
+    <mergeCell ref="YW51:YX51"/>
+    <mergeCell ref="ZB51:ZP51"/>
+    <mergeCell ref="WY51:WZ51"/>
+    <mergeCell ref="XD51:XR51"/>
+    <mergeCell ref="XS51:XT51"/>
+    <mergeCell ref="XU51:XV51"/>
+    <mergeCell ref="XX51:XY51"/>
+    <mergeCell ref="VW51:VX51"/>
+    <mergeCell ref="VZ51:WA51"/>
+    <mergeCell ref="WE51:WS51"/>
+    <mergeCell ref="WT51:WU51"/>
+    <mergeCell ref="WV51:WW51"/>
+    <mergeCell ref="UV51:UW51"/>
+    <mergeCell ref="UX51:UY51"/>
+    <mergeCell ref="VA51:VB51"/>
+    <mergeCell ref="VF51:VT51"/>
+    <mergeCell ref="VU51:VV51"/>
+    <mergeCell ref="TW51:TX51"/>
+    <mergeCell ref="TY51:TZ51"/>
+    <mergeCell ref="UB51:UC51"/>
+    <mergeCell ref="UG51:UU51"/>
+    <mergeCell ref="SD51:SE51"/>
+    <mergeCell ref="SI51:SW51"/>
+    <mergeCell ref="SX51:SY51"/>
+    <mergeCell ref="SZ51:TA51"/>
+    <mergeCell ref="TC51:TD51"/>
+    <mergeCell ref="UH39:UI40"/>
+    <mergeCell ref="UT39:UU40"/>
+    <mergeCell ref="VG39:VH40"/>
+    <mergeCell ref="VS39:VT40"/>
+    <mergeCell ref="WF39:WG40"/>
+    <mergeCell ref="AAB39:AAC40"/>
+    <mergeCell ref="AAN39:AAO40"/>
+    <mergeCell ref="ABA39:ABB40"/>
+    <mergeCell ref="WR39:WS40"/>
+    <mergeCell ref="XE39:XF40"/>
+    <mergeCell ref="XQ39:XR40"/>
+    <mergeCell ref="YD39:YE40"/>
+    <mergeCell ref="YP39:YQ40"/>
+    <mergeCell ref="OM51:PA51"/>
+    <mergeCell ref="PB51:PC51"/>
+    <mergeCell ref="PD51:PE51"/>
+    <mergeCell ref="PG51:PH51"/>
+    <mergeCell ref="PL51:PZ51"/>
+    <mergeCell ref="RB51:RC51"/>
+    <mergeCell ref="RE51:RF51"/>
+    <mergeCell ref="RJ51:RX51"/>
+    <mergeCell ref="RY51:RZ51"/>
+    <mergeCell ref="ON39:OO40"/>
+    <mergeCell ref="OZ39:PA40"/>
+    <mergeCell ref="PM39:PN40"/>
+    <mergeCell ref="PY39:PZ40"/>
+    <mergeCell ref="QL39:QM40"/>
+    <mergeCell ref="QX39:QY40"/>
+    <mergeCell ref="RK39:RL40"/>
+    <mergeCell ref="RW39:RX40"/>
+    <mergeCell ref="SJ39:SK40"/>
+    <mergeCell ref="ADK39:ADL40"/>
+    <mergeCell ref="ZC39:ZD40"/>
+    <mergeCell ref="ZO39:ZP40"/>
+    <mergeCell ref="YP27:YQ28"/>
+    <mergeCell ref="ZC27:ZD28"/>
+    <mergeCell ref="SA51:SB51"/>
+    <mergeCell ref="QA51:QB51"/>
+    <mergeCell ref="QC51:QD51"/>
+    <mergeCell ref="QF51:QG51"/>
+    <mergeCell ref="QK51:QY51"/>
+    <mergeCell ref="QZ51:RA51"/>
+    <mergeCell ref="TH51:TV51"/>
+    <mergeCell ref="ADK27:ADL28"/>
+    <mergeCell ref="SV39:SW40"/>
+    <mergeCell ref="TI39:TJ40"/>
+    <mergeCell ref="TU39:TV40"/>
+    <mergeCell ref="ZO27:ZP28"/>
+    <mergeCell ref="AAB27:AAC28"/>
+    <mergeCell ref="AAN27:AAO28"/>
+    <mergeCell ref="ABA27:ABB28"/>
+    <mergeCell ref="ABM39:ABN40"/>
+    <mergeCell ref="ABZ39:ACA40"/>
+    <mergeCell ref="ACL39:ACM40"/>
+    <mergeCell ref="ACY39:ACZ40"/>
+    <mergeCell ref="UT27:UU28"/>
+    <mergeCell ref="VG27:VH28"/>
+    <mergeCell ref="VS27:VT28"/>
+    <mergeCell ref="WF27:WG28"/>
+    <mergeCell ref="WR27:WS28"/>
+    <mergeCell ref="ACL15:ACM16"/>
+    <mergeCell ref="ACY15:ACZ16"/>
+    <mergeCell ref="VG15:VH16"/>
+    <mergeCell ref="VS15:VT16"/>
+    <mergeCell ref="WF15:WG16"/>
+    <mergeCell ref="WR15:WS16"/>
+    <mergeCell ref="XE15:XF16"/>
+    <mergeCell ref="ABZ27:ACA28"/>
+    <mergeCell ref="ACL27:ACM28"/>
+    <mergeCell ref="ACY27:ACZ28"/>
+    <mergeCell ref="ABM27:ABN28"/>
+    <mergeCell ref="XE27:XF28"/>
+    <mergeCell ref="XQ27:XR28"/>
+    <mergeCell ref="YD27:YE28"/>
+    <mergeCell ref="ADK15:ADL16"/>
+    <mergeCell ref="ON27:OO28"/>
+    <mergeCell ref="OZ27:PA28"/>
+    <mergeCell ref="PM27:PN28"/>
+    <mergeCell ref="PY27:PZ28"/>
+    <mergeCell ref="QL27:QM28"/>
+    <mergeCell ref="QX27:QY28"/>
+    <mergeCell ref="RK27:RL28"/>
+    <mergeCell ref="RW27:RX28"/>
+    <mergeCell ref="SJ27:SK28"/>
+    <mergeCell ref="SV27:SW28"/>
+    <mergeCell ref="TI27:TJ28"/>
+    <mergeCell ref="TU27:TV28"/>
+    <mergeCell ref="UH27:UI28"/>
+    <mergeCell ref="AAB15:AAC16"/>
+    <mergeCell ref="AAN15:AAO16"/>
+    <mergeCell ref="ABA15:ABB16"/>
+    <mergeCell ref="ABM15:ABN16"/>
+    <mergeCell ref="ABZ15:ACA16"/>
+    <mergeCell ref="XQ15:XR16"/>
+    <mergeCell ref="YD15:YE16"/>
+    <mergeCell ref="YP15:YQ16"/>
+    <mergeCell ref="ZC15:ZD16"/>
+    <mergeCell ref="ZO15:ZP16"/>
+    <mergeCell ref="ACY3:ACZ4"/>
+    <mergeCell ref="ADK3:ADL4"/>
+    <mergeCell ref="ON15:OO16"/>
+    <mergeCell ref="OZ15:PA16"/>
+    <mergeCell ref="PM15:PN16"/>
+    <mergeCell ref="PY15:PZ16"/>
+    <mergeCell ref="QL15:QM16"/>
+    <mergeCell ref="QX15:QY16"/>
+    <mergeCell ref="RK15:RL16"/>
+    <mergeCell ref="RW15:RX16"/>
+    <mergeCell ref="SJ15:SK16"/>
+    <mergeCell ref="SV15:SW16"/>
+    <mergeCell ref="TI15:TJ16"/>
+    <mergeCell ref="TU15:TV16"/>
+    <mergeCell ref="UH15:UI16"/>
+    <mergeCell ref="UT15:UU16"/>
+    <mergeCell ref="AAN3:AAO4"/>
+    <mergeCell ref="ABA3:ABB4"/>
+    <mergeCell ref="ABM3:ABN4"/>
+    <mergeCell ref="ABZ3:ACA4"/>
+    <mergeCell ref="ACL3:ACM4"/>
+    <mergeCell ref="YD3:YE4"/>
+    <mergeCell ref="YP3:YQ4"/>
+    <mergeCell ref="ZC3:ZD4"/>
+    <mergeCell ref="ZO3:ZP4"/>
+    <mergeCell ref="AAB3:AAC4"/>
+    <mergeCell ref="VS3:VT4"/>
+    <mergeCell ref="WF3:WG4"/>
+    <mergeCell ref="WR3:WS4"/>
+    <mergeCell ref="XE3:XF4"/>
+    <mergeCell ref="XQ3:XR4"/>
+    <mergeCell ref="TI3:TJ4"/>
+    <mergeCell ref="TU3:TV4"/>
+    <mergeCell ref="UH3:UI4"/>
+    <mergeCell ref="UT3:UU4"/>
+    <mergeCell ref="VG3:VH4"/>
+    <mergeCell ref="QX3:QY4"/>
+    <mergeCell ref="RK3:RL4"/>
+    <mergeCell ref="RW3:RX4"/>
+    <mergeCell ref="SJ3:SK4"/>
+    <mergeCell ref="SV3:SW4"/>
+    <mergeCell ref="ON3:OO4"/>
+    <mergeCell ref="OZ3:PA4"/>
+    <mergeCell ref="PM3:PN4"/>
+    <mergeCell ref="PY3:PZ4"/>
+    <mergeCell ref="QL3:QM4"/>
+    <mergeCell ref="NI51:NJ51"/>
+    <mergeCell ref="NN51:OB51"/>
+    <mergeCell ref="OC51:OD51"/>
+    <mergeCell ref="OE51:OF51"/>
+    <mergeCell ref="OH51:OI51"/>
+    <mergeCell ref="MG51:MH51"/>
+    <mergeCell ref="MJ51:MK51"/>
+    <mergeCell ref="MO51:NC51"/>
+    <mergeCell ref="ND51:NE51"/>
+    <mergeCell ref="NF51:NG51"/>
+    <mergeCell ref="NO39:NP40"/>
+    <mergeCell ref="OA39:OB40"/>
+    <mergeCell ref="GU51:HI51"/>
+    <mergeCell ref="HJ51:HK51"/>
+    <mergeCell ref="HL51:HM51"/>
+    <mergeCell ref="HO51:HP51"/>
+    <mergeCell ref="HT51:IH51"/>
+    <mergeCell ref="II51:IJ51"/>
+    <mergeCell ref="IK51:IL51"/>
+    <mergeCell ref="IN51:IO51"/>
+    <mergeCell ref="IS51:JG51"/>
+    <mergeCell ref="JH51:JI51"/>
+    <mergeCell ref="JJ51:JK51"/>
+    <mergeCell ref="JM51:JN51"/>
+    <mergeCell ref="LF51:LG51"/>
+    <mergeCell ref="LH51:LI51"/>
+    <mergeCell ref="LK51:LL51"/>
+    <mergeCell ref="LP51:MD51"/>
+    <mergeCell ref="ME51:MF51"/>
+    <mergeCell ref="JR51:KF51"/>
+    <mergeCell ref="KG51:KH51"/>
+    <mergeCell ref="KI51:KJ51"/>
+    <mergeCell ref="KL51:KM51"/>
+    <mergeCell ref="KQ51:LE51"/>
+    <mergeCell ref="JF39:JG40"/>
+    <mergeCell ref="JS39:JT40"/>
+    <mergeCell ref="KE39:KF40"/>
+    <mergeCell ref="KR39:KS40"/>
+    <mergeCell ref="LD39:LE40"/>
+    <mergeCell ref="LQ39:LR40"/>
+    <mergeCell ref="MC39:MD40"/>
+    <mergeCell ref="MP39:MQ40"/>
+    <mergeCell ref="NB39:NC40"/>
+    <mergeCell ref="MP15:MQ16"/>
+    <mergeCell ref="NB15:NC16"/>
+    <mergeCell ref="NO15:NP16"/>
+    <mergeCell ref="OA15:OB16"/>
+    <mergeCell ref="GV27:GW28"/>
+    <mergeCell ref="HH27:HI28"/>
+    <mergeCell ref="HU27:HV28"/>
+    <mergeCell ref="IG27:IH28"/>
+    <mergeCell ref="IT27:IU28"/>
+    <mergeCell ref="JF27:JG28"/>
+    <mergeCell ref="JS27:JT28"/>
+    <mergeCell ref="KE27:KF28"/>
+    <mergeCell ref="KR27:KS28"/>
+    <mergeCell ref="LD27:LE28"/>
+    <mergeCell ref="LQ27:LR28"/>
+    <mergeCell ref="MC27:MD28"/>
+    <mergeCell ref="MP27:MQ28"/>
+    <mergeCell ref="NB27:NC28"/>
+    <mergeCell ref="NO27:NP28"/>
+    <mergeCell ref="OA27:OB28"/>
+    <mergeCell ref="MP3:MQ4"/>
+    <mergeCell ref="NB3:NC4"/>
+    <mergeCell ref="NO3:NP4"/>
+    <mergeCell ref="OA3:OB4"/>
+    <mergeCell ref="GV15:GW16"/>
+    <mergeCell ref="HH15:HI16"/>
+    <mergeCell ref="HU15:HV16"/>
+    <mergeCell ref="IG15:IH16"/>
+    <mergeCell ref="IT15:IU16"/>
+    <mergeCell ref="JF15:JG16"/>
+    <mergeCell ref="JS15:JT16"/>
+    <mergeCell ref="KE15:KF16"/>
+    <mergeCell ref="KR15:KS16"/>
+    <mergeCell ref="LD15:LE16"/>
+    <mergeCell ref="LQ15:LR16"/>
+    <mergeCell ref="MC15:MD16"/>
+    <mergeCell ref="KE3:KF4"/>
+    <mergeCell ref="KR3:KS4"/>
+    <mergeCell ref="LD3:LE4"/>
+    <mergeCell ref="LQ3:LR4"/>
+    <mergeCell ref="MC3:MD4"/>
+    <mergeCell ref="HU3:HV4"/>
+    <mergeCell ref="IG3:IH4"/>
+    <mergeCell ref="IT3:IU4"/>
     <mergeCell ref="JF3:JG4"/>
     <mergeCell ref="JS3:JT4"/>
     <mergeCell ref="GK51:GL51"/>
@@ -43837,285 +44330,87 @@
     <mergeCell ref="HU39:HV40"/>
     <mergeCell ref="IG39:IH40"/>
     <mergeCell ref="IT39:IU40"/>
-    <mergeCell ref="MP3:MQ4"/>
-    <mergeCell ref="NB3:NC4"/>
-    <mergeCell ref="NO3:NP4"/>
-    <mergeCell ref="OA3:OB4"/>
-    <mergeCell ref="GV15:GW16"/>
-    <mergeCell ref="HH15:HI16"/>
-    <mergeCell ref="HU15:HV16"/>
-    <mergeCell ref="IG15:IH16"/>
-    <mergeCell ref="IT15:IU16"/>
-    <mergeCell ref="JF15:JG16"/>
-    <mergeCell ref="JS15:JT16"/>
-    <mergeCell ref="KE15:KF16"/>
-    <mergeCell ref="KR15:KS16"/>
-    <mergeCell ref="LD15:LE16"/>
-    <mergeCell ref="LQ15:LR16"/>
-    <mergeCell ref="MC15:MD16"/>
-    <mergeCell ref="KE3:KF4"/>
-    <mergeCell ref="KR3:KS4"/>
-    <mergeCell ref="LD3:LE4"/>
-    <mergeCell ref="LQ3:LR4"/>
-    <mergeCell ref="MC3:MD4"/>
-    <mergeCell ref="HU3:HV4"/>
-    <mergeCell ref="IG3:IH4"/>
-    <mergeCell ref="IT3:IU4"/>
-    <mergeCell ref="MP15:MQ16"/>
-    <mergeCell ref="NB15:NC16"/>
-    <mergeCell ref="NO15:NP16"/>
-    <mergeCell ref="OA15:OB16"/>
-    <mergeCell ref="GV27:GW28"/>
-    <mergeCell ref="HH27:HI28"/>
-    <mergeCell ref="HU27:HV28"/>
-    <mergeCell ref="IG27:IH28"/>
-    <mergeCell ref="IT27:IU28"/>
-    <mergeCell ref="JF27:JG28"/>
-    <mergeCell ref="JS27:JT28"/>
-    <mergeCell ref="KE27:KF28"/>
-    <mergeCell ref="KR27:KS28"/>
-    <mergeCell ref="LD27:LE28"/>
-    <mergeCell ref="LQ27:LR28"/>
-    <mergeCell ref="MC27:MD28"/>
-    <mergeCell ref="MP27:MQ28"/>
-    <mergeCell ref="NB27:NC28"/>
-    <mergeCell ref="NO27:NP28"/>
-    <mergeCell ref="OA27:OB28"/>
-    <mergeCell ref="JF39:JG40"/>
-    <mergeCell ref="JS39:JT40"/>
-    <mergeCell ref="KE39:KF40"/>
-    <mergeCell ref="KR39:KS40"/>
-    <mergeCell ref="LD39:LE40"/>
-    <mergeCell ref="LQ39:LR40"/>
-    <mergeCell ref="MC39:MD40"/>
-    <mergeCell ref="MP39:MQ40"/>
-    <mergeCell ref="NB39:NC40"/>
-    <mergeCell ref="NO39:NP40"/>
-    <mergeCell ref="OA39:OB40"/>
-    <mergeCell ref="GU51:HI51"/>
-    <mergeCell ref="HJ51:HK51"/>
-    <mergeCell ref="HL51:HM51"/>
-    <mergeCell ref="HO51:HP51"/>
-    <mergeCell ref="HT51:IH51"/>
-    <mergeCell ref="II51:IJ51"/>
-    <mergeCell ref="IK51:IL51"/>
-    <mergeCell ref="IN51:IO51"/>
-    <mergeCell ref="IS51:JG51"/>
-    <mergeCell ref="JH51:JI51"/>
-    <mergeCell ref="JJ51:JK51"/>
-    <mergeCell ref="JM51:JN51"/>
-    <mergeCell ref="LF51:LG51"/>
-    <mergeCell ref="LH51:LI51"/>
-    <mergeCell ref="LK51:LL51"/>
-    <mergeCell ref="LP51:MD51"/>
-    <mergeCell ref="ME51:MF51"/>
-    <mergeCell ref="JR51:KF51"/>
-    <mergeCell ref="KG51:KH51"/>
-    <mergeCell ref="KI51:KJ51"/>
-    <mergeCell ref="KL51:KM51"/>
-    <mergeCell ref="KQ51:LE51"/>
-    <mergeCell ref="NI51:NJ51"/>
-    <mergeCell ref="NN51:OB51"/>
-    <mergeCell ref="OC51:OD51"/>
-    <mergeCell ref="OE51:OF51"/>
-    <mergeCell ref="OH51:OI51"/>
-    <mergeCell ref="MG51:MH51"/>
-    <mergeCell ref="MJ51:MK51"/>
-    <mergeCell ref="MO51:NC51"/>
-    <mergeCell ref="ND51:NE51"/>
-    <mergeCell ref="NF51:NG51"/>
-    <mergeCell ref="QX3:QY4"/>
-    <mergeCell ref="RK3:RL4"/>
-    <mergeCell ref="RW3:RX4"/>
-    <mergeCell ref="SJ3:SK4"/>
-    <mergeCell ref="SV3:SW4"/>
-    <mergeCell ref="ON3:OO4"/>
-    <mergeCell ref="OZ3:PA4"/>
-    <mergeCell ref="PM3:PN4"/>
-    <mergeCell ref="PY3:PZ4"/>
-    <mergeCell ref="QL3:QM4"/>
-    <mergeCell ref="ZO3:ZP4"/>
-    <mergeCell ref="AAB3:AAC4"/>
-    <mergeCell ref="VS3:VT4"/>
-    <mergeCell ref="WF3:WG4"/>
-    <mergeCell ref="WR3:WS4"/>
-    <mergeCell ref="XE3:XF4"/>
-    <mergeCell ref="XQ3:XR4"/>
-    <mergeCell ref="TI3:TJ4"/>
-    <mergeCell ref="TU3:TV4"/>
-    <mergeCell ref="UH3:UI4"/>
-    <mergeCell ref="UT3:UU4"/>
-    <mergeCell ref="VG3:VH4"/>
-    <mergeCell ref="ACY3:ACZ4"/>
-    <mergeCell ref="ADK3:ADL4"/>
-    <mergeCell ref="ON15:OO16"/>
-    <mergeCell ref="OZ15:PA16"/>
-    <mergeCell ref="PM15:PN16"/>
-    <mergeCell ref="PY15:PZ16"/>
-    <mergeCell ref="QL15:QM16"/>
-    <mergeCell ref="QX15:QY16"/>
-    <mergeCell ref="RK15:RL16"/>
-    <mergeCell ref="RW15:RX16"/>
-    <mergeCell ref="SJ15:SK16"/>
-    <mergeCell ref="SV15:SW16"/>
-    <mergeCell ref="TI15:TJ16"/>
-    <mergeCell ref="TU15:TV16"/>
-    <mergeCell ref="UH15:UI16"/>
-    <mergeCell ref="UT15:UU16"/>
-    <mergeCell ref="AAN3:AAO4"/>
-    <mergeCell ref="ABA3:ABB4"/>
-    <mergeCell ref="ABM3:ABN4"/>
-    <mergeCell ref="ABZ3:ACA4"/>
-    <mergeCell ref="ACL3:ACM4"/>
-    <mergeCell ref="YD3:YE4"/>
-    <mergeCell ref="YP3:YQ4"/>
-    <mergeCell ref="ZC3:ZD4"/>
-    <mergeCell ref="ADK15:ADL16"/>
-    <mergeCell ref="ON27:OO28"/>
-    <mergeCell ref="OZ27:PA28"/>
-    <mergeCell ref="PM27:PN28"/>
-    <mergeCell ref="PY27:PZ28"/>
-    <mergeCell ref="QL27:QM28"/>
-    <mergeCell ref="QX27:QY28"/>
-    <mergeCell ref="RK27:RL28"/>
-    <mergeCell ref="RW27:RX28"/>
-    <mergeCell ref="SJ27:SK28"/>
-    <mergeCell ref="SV27:SW28"/>
-    <mergeCell ref="TI27:TJ28"/>
-    <mergeCell ref="TU27:TV28"/>
-    <mergeCell ref="UH27:UI28"/>
-    <mergeCell ref="AAB15:AAC16"/>
-    <mergeCell ref="AAN15:AAO16"/>
-    <mergeCell ref="ABA15:ABB16"/>
-    <mergeCell ref="ABM15:ABN16"/>
-    <mergeCell ref="ABZ15:ACA16"/>
-    <mergeCell ref="XQ15:XR16"/>
-    <mergeCell ref="YD15:YE16"/>
-    <mergeCell ref="YP15:YQ16"/>
-    <mergeCell ref="ZC15:ZD16"/>
-    <mergeCell ref="ZO15:ZP16"/>
-    <mergeCell ref="UT27:UU28"/>
-    <mergeCell ref="VG27:VH28"/>
-    <mergeCell ref="VS27:VT28"/>
-    <mergeCell ref="WF27:WG28"/>
-    <mergeCell ref="WR27:WS28"/>
-    <mergeCell ref="ACL15:ACM16"/>
-    <mergeCell ref="ACY15:ACZ16"/>
-    <mergeCell ref="VG15:VH16"/>
-    <mergeCell ref="VS15:VT16"/>
-    <mergeCell ref="WF15:WG16"/>
-    <mergeCell ref="WR15:WS16"/>
-    <mergeCell ref="XE15:XF16"/>
-    <mergeCell ref="ABZ27:ACA28"/>
-    <mergeCell ref="ACL27:ACM28"/>
-    <mergeCell ref="ACY27:ACZ28"/>
-    <mergeCell ref="ABM27:ABN28"/>
-    <mergeCell ref="XE27:XF28"/>
-    <mergeCell ref="XQ27:XR28"/>
-    <mergeCell ref="YD27:YE28"/>
-    <mergeCell ref="ADK39:ADL40"/>
-    <mergeCell ref="ZC39:ZD40"/>
-    <mergeCell ref="ZO39:ZP40"/>
-    <mergeCell ref="YP27:YQ28"/>
-    <mergeCell ref="ZC27:ZD28"/>
-    <mergeCell ref="SA51:SB51"/>
-    <mergeCell ref="QA51:QB51"/>
-    <mergeCell ref="QC51:QD51"/>
-    <mergeCell ref="QF51:QG51"/>
-    <mergeCell ref="QK51:QY51"/>
-    <mergeCell ref="QZ51:RA51"/>
-    <mergeCell ref="TH51:TV51"/>
-    <mergeCell ref="ADK27:ADL28"/>
-    <mergeCell ref="SV39:SW40"/>
-    <mergeCell ref="TI39:TJ40"/>
-    <mergeCell ref="TU39:TV40"/>
-    <mergeCell ref="ZO27:ZP28"/>
-    <mergeCell ref="AAB27:AAC28"/>
-    <mergeCell ref="AAN27:AAO28"/>
-    <mergeCell ref="ABA27:ABB28"/>
-    <mergeCell ref="ABM39:ABN40"/>
-    <mergeCell ref="ABZ39:ACA40"/>
-    <mergeCell ref="ACL39:ACM40"/>
-    <mergeCell ref="ACY39:ACZ40"/>
-    <mergeCell ref="ON39:OO40"/>
-    <mergeCell ref="OZ39:PA40"/>
-    <mergeCell ref="PM39:PN40"/>
-    <mergeCell ref="PY39:PZ40"/>
-    <mergeCell ref="QL39:QM40"/>
-    <mergeCell ref="QX39:QY40"/>
-    <mergeCell ref="RK39:RL40"/>
-    <mergeCell ref="RW39:RX40"/>
-    <mergeCell ref="SJ39:SK40"/>
-    <mergeCell ref="OM51:PA51"/>
-    <mergeCell ref="PB51:PC51"/>
-    <mergeCell ref="PD51:PE51"/>
-    <mergeCell ref="PG51:PH51"/>
-    <mergeCell ref="PL51:PZ51"/>
-    <mergeCell ref="RB51:RC51"/>
-    <mergeCell ref="RE51:RF51"/>
-    <mergeCell ref="RJ51:RX51"/>
-    <mergeCell ref="RY51:RZ51"/>
-    <mergeCell ref="UH39:UI40"/>
-    <mergeCell ref="UT39:UU40"/>
-    <mergeCell ref="VG39:VH40"/>
-    <mergeCell ref="VS39:VT40"/>
-    <mergeCell ref="WF39:WG40"/>
-    <mergeCell ref="AAB39:AAC40"/>
-    <mergeCell ref="AAN39:AAO40"/>
-    <mergeCell ref="ABA39:ABB40"/>
-    <mergeCell ref="WR39:WS40"/>
-    <mergeCell ref="XE39:XF40"/>
-    <mergeCell ref="XQ39:XR40"/>
-    <mergeCell ref="YD39:YE40"/>
-    <mergeCell ref="YP39:YQ40"/>
-    <mergeCell ref="TW51:TX51"/>
-    <mergeCell ref="TY51:TZ51"/>
-    <mergeCell ref="UB51:UC51"/>
-    <mergeCell ref="UG51:UU51"/>
-    <mergeCell ref="SD51:SE51"/>
-    <mergeCell ref="SI51:SW51"/>
-    <mergeCell ref="SX51:SY51"/>
-    <mergeCell ref="SZ51:TA51"/>
-    <mergeCell ref="TC51:TD51"/>
-    <mergeCell ref="VW51:VX51"/>
-    <mergeCell ref="VZ51:WA51"/>
-    <mergeCell ref="WE51:WS51"/>
-    <mergeCell ref="WT51:WU51"/>
-    <mergeCell ref="WV51:WW51"/>
-    <mergeCell ref="UV51:UW51"/>
-    <mergeCell ref="UX51:UY51"/>
-    <mergeCell ref="VA51:VB51"/>
-    <mergeCell ref="VF51:VT51"/>
-    <mergeCell ref="VU51:VV51"/>
-    <mergeCell ref="YC51:YQ51"/>
-    <mergeCell ref="YR51:YS51"/>
-    <mergeCell ref="YT51:YU51"/>
-    <mergeCell ref="YW51:YX51"/>
-    <mergeCell ref="ZB51:ZP51"/>
-    <mergeCell ref="WY51:WZ51"/>
-    <mergeCell ref="XD51:XR51"/>
-    <mergeCell ref="XS51:XT51"/>
-    <mergeCell ref="XU51:XV51"/>
-    <mergeCell ref="XX51:XY51"/>
-    <mergeCell ref="AAR51:AAS51"/>
-    <mergeCell ref="AAU51:AAV51"/>
-    <mergeCell ref="AAZ51:ABN51"/>
-    <mergeCell ref="ABO51:ABP51"/>
-    <mergeCell ref="ABQ51:ABR51"/>
-    <mergeCell ref="ZQ51:ZR51"/>
-    <mergeCell ref="ZS51:ZT51"/>
-    <mergeCell ref="ZV51:ZW51"/>
-    <mergeCell ref="AAA51:AAO51"/>
-    <mergeCell ref="AAP51:AAQ51"/>
-    <mergeCell ref="ACX51:ADL51"/>
-    <mergeCell ref="ADM51:ADN51"/>
-    <mergeCell ref="ADO51:ADP51"/>
-    <mergeCell ref="ADR51:ADS51"/>
-    <mergeCell ref="ABT51:ABU51"/>
-    <mergeCell ref="ABY51:ACM51"/>
-    <mergeCell ref="ACN51:ACO51"/>
-    <mergeCell ref="ACP51:ACQ51"/>
-    <mergeCell ref="ACS51:ACT51"/>
+    <mergeCell ref="EM51:EN51"/>
+    <mergeCell ref="EO51:EP51"/>
+    <mergeCell ref="ER51:ES51"/>
+    <mergeCell ref="EX3:EY4"/>
+    <mergeCell ref="FJ3:FK4"/>
+    <mergeCell ref="EX15:EY16"/>
+    <mergeCell ref="FJ15:FK16"/>
+    <mergeCell ref="EX27:EY28"/>
+    <mergeCell ref="FJ27:FK28"/>
+    <mergeCell ref="EX39:EY40"/>
+    <mergeCell ref="FJ39:FK40"/>
+    <mergeCell ref="EW51:FK51"/>
+    <mergeCell ref="DN51:DO51"/>
+    <mergeCell ref="DP51:DQ51"/>
+    <mergeCell ref="DS51:DT51"/>
+    <mergeCell ref="DY3:DZ4"/>
+    <mergeCell ref="EK3:EL4"/>
+    <mergeCell ref="DY15:DZ16"/>
+    <mergeCell ref="EK15:EL16"/>
+    <mergeCell ref="DY27:DZ28"/>
+    <mergeCell ref="EK27:EL28"/>
+    <mergeCell ref="DY39:DZ40"/>
+    <mergeCell ref="EK39:EL40"/>
+    <mergeCell ref="DX51:EL51"/>
+    <mergeCell ref="CO51:CP51"/>
+    <mergeCell ref="CQ51:CR51"/>
+    <mergeCell ref="CT51:CU51"/>
+    <mergeCell ref="CZ3:DA4"/>
+    <mergeCell ref="DL3:DM4"/>
+    <mergeCell ref="CZ15:DA16"/>
+    <mergeCell ref="DL15:DM16"/>
+    <mergeCell ref="CZ27:DA28"/>
+    <mergeCell ref="DL27:DM28"/>
+    <mergeCell ref="CZ39:DA40"/>
+    <mergeCell ref="DL39:DM40"/>
+    <mergeCell ref="CY51:DM51"/>
+    <mergeCell ref="BU51:BV51"/>
+    <mergeCell ref="CA3:CB4"/>
+    <mergeCell ref="CM3:CN4"/>
+    <mergeCell ref="CA15:CB16"/>
+    <mergeCell ref="CM15:CN16"/>
+    <mergeCell ref="CA27:CB28"/>
+    <mergeCell ref="CM27:CN28"/>
+    <mergeCell ref="CA39:CB40"/>
+    <mergeCell ref="CM39:CN40"/>
+    <mergeCell ref="BZ51:CN51"/>
+    <mergeCell ref="BB39:BC40"/>
+    <mergeCell ref="BN39:BO40"/>
+    <mergeCell ref="BA51:BO51"/>
+    <mergeCell ref="BP51:BQ51"/>
+    <mergeCell ref="BR51:BS51"/>
+    <mergeCell ref="BB3:BC4"/>
+    <mergeCell ref="BN3:BO4"/>
+    <mergeCell ref="BB15:BC16"/>
+    <mergeCell ref="BN15:BO16"/>
+    <mergeCell ref="BB27:BC28"/>
+    <mergeCell ref="BN27:BO28"/>
+    <mergeCell ref="AO39:AP40"/>
+    <mergeCell ref="AB51:AP51"/>
+    <mergeCell ref="AQ51:AR51"/>
+    <mergeCell ref="AS51:AT51"/>
+    <mergeCell ref="AV51:AW51"/>
+    <mergeCell ref="AO3:AP4"/>
+    <mergeCell ref="AC15:AD16"/>
+    <mergeCell ref="AO15:AP16"/>
+    <mergeCell ref="AC27:AD28"/>
+    <mergeCell ref="AO27:AP28"/>
+    <mergeCell ref="C51:Q51"/>
+    <mergeCell ref="R51:S51"/>
+    <mergeCell ref="T51:U51"/>
+    <mergeCell ref="W51:X51"/>
+    <mergeCell ref="AC3:AD4"/>
+    <mergeCell ref="AC39:AD40"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="P3:Q4"/>
+    <mergeCell ref="D39:E40"/>
+    <mergeCell ref="P39:Q40"/>
+    <mergeCell ref="P27:Q28"/>
+    <mergeCell ref="D27:E28"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="P15:Q16"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -44245,46 +44540,46 @@
     <row r="4" spans="1:37" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="102"/>
+      <c r="D4" s="100"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="102" t="s">
+      <c r="F4" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
       <c r="J4" s="37"/>
       <c r="K4" s="37"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="102" t="s">
+      <c r="M4" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="102"/>
+      <c r="N4" s="100"/>
       <c r="O4" s="2"/>
       <c r="P4" s="36"/>
       <c r="Q4" s="36"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="102" t="s">
+      <c r="S4" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="102"/>
+      <c r="T4" s="100"/>
       <c r="U4" s="6"/>
-      <c r="V4" s="102" t="s">
+      <c r="V4" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="W4" s="102"/>
-      <c r="X4" s="102"/>
-      <c r="Y4" s="102"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="100"/>
+      <c r="Y4" s="100"/>
       <c r="Z4" s="37"/>
       <c r="AA4" s="37"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="102" t="s">
+      <c r="AC4" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" s="102"/>
+      <c r="AD4" s="100"/>
     </row>
     <row r="5" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -44313,10 +44608,10 @@
     <row r="6" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="100"/>
+      <c r="D6" s="101"/>
       <c r="E6" s="5"/>
       <c r="F6" s="7">
         <v>0</v>
@@ -44335,18 +44630,18 @@
         <v>23</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="101">
+      <c r="M6" s="102">
         <v>0</v>
       </c>
-      <c r="N6" s="101"/>
+      <c r="N6" s="102"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
-      <c r="S6" s="100" t="s">
+      <c r="S6" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="T6" s="100"/>
+      <c r="T6" s="101"/>
       <c r="U6" s="5"/>
       <c r="V6" s="7">
         <v>1</v>
@@ -44365,18 +44660,18 @@
         <v>23</v>
       </c>
       <c r="AB6" s="3"/>
-      <c r="AC6" s="101">
+      <c r="AC6" s="102">
         <v>8</v>
       </c>
-      <c r="AD6" s="101"/>
+      <c r="AD6" s="102"/>
     </row>
     <row r="7" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="100"/>
+      <c r="D7" s="101"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7">
         <v>0</v>
@@ -44395,18 +44690,18 @@
         <v>23</v>
       </c>
       <c r="L7" s="3"/>
-      <c r="M7" s="101">
+      <c r="M7" s="102">
         <v>1</v>
       </c>
-      <c r="N7" s="101"/>
+      <c r="N7" s="102"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="100" t="s">
+      <c r="S7" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="T7" s="100"/>
+      <c r="T7" s="101"/>
       <c r="U7" s="5"/>
       <c r="V7" s="7">
         <v>1</v>
@@ -44425,18 +44720,18 @@
         <v>23</v>
       </c>
       <c r="AB7" s="3"/>
-      <c r="AC7" s="101">
+      <c r="AC7" s="102">
         <v>9</v>
       </c>
-      <c r="AD7" s="101"/>
+      <c r="AD7" s="102"/>
     </row>
     <row r="8" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="100"/>
+      <c r="D8" s="101"/>
       <c r="E8" s="5"/>
       <c r="F8" s="7">
         <v>0</v>
@@ -44455,18 +44750,18 @@
         <v>23</v>
       </c>
       <c r="L8" s="3"/>
-      <c r="M8" s="101">
+      <c r="M8" s="102">
         <v>2</v>
       </c>
-      <c r="N8" s="101"/>
+      <c r="N8" s="102"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="100">
+      <c r="S8" s="101">
         <v>10</v>
       </c>
-      <c r="T8" s="100"/>
+      <c r="T8" s="101"/>
       <c r="U8" s="5"/>
       <c r="V8" s="7">
         <v>1</v>
@@ -44485,18 +44780,18 @@
         <v>23</v>
       </c>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="101" t="s">
+      <c r="AC8" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="AD8" s="101"/>
+      <c r="AD8" s="102"/>
     </row>
     <row r="9" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="100"/>
+      <c r="D9" s="101"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7">
         <v>0</v>
@@ -44515,18 +44810,18 @@
         <v>23</v>
       </c>
       <c r="L9" s="3"/>
-      <c r="M9" s="101">
+      <c r="M9" s="102">
         <v>3</v>
       </c>
-      <c r="N9" s="101"/>
+      <c r="N9" s="102"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="100" t="s">
+      <c r="S9" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="100"/>
+      <c r="T9" s="101"/>
       <c r="U9" s="5"/>
       <c r="V9" s="7">
         <v>1</v>
@@ -44545,18 +44840,18 @@
         <v>23</v>
       </c>
       <c r="AB9" s="3"/>
-      <c r="AC9" s="101" t="s">
+      <c r="AC9" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="AD9" s="101"/>
+      <c r="AD9" s="102"/>
     </row>
     <row r="10" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="100" t="s">
+      <c r="C10" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="100"/>
+      <c r="D10" s="101"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7">
         <v>0</v>
@@ -44575,18 +44870,18 @@
         <v>23</v>
       </c>
       <c r="L10" s="3"/>
-      <c r="M10" s="101">
+      <c r="M10" s="102">
         <v>4</v>
       </c>
-      <c r="N10" s="101"/>
+      <c r="N10" s="102"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="100" t="s">
+      <c r="S10" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="T10" s="100"/>
+      <c r="T10" s="101"/>
       <c r="U10" s="5"/>
       <c r="V10" s="7">
         <v>1</v>
@@ -44605,18 +44900,18 @@
         <v>23</v>
       </c>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="101" t="s">
+      <c r="AC10" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="AD10" s="101"/>
+      <c r="AD10" s="102"/>
     </row>
     <row r="11" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="100"/>
+      <c r="D11" s="101"/>
       <c r="E11" s="5"/>
       <c r="F11" s="7">
         <v>0</v>
@@ -44635,18 +44930,18 @@
         <v>23</v>
       </c>
       <c r="L11" s="3"/>
-      <c r="M11" s="101">
+      <c r="M11" s="102">
         <v>5</v>
       </c>
-      <c r="N11" s="101"/>
+      <c r="N11" s="102"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="100" t="s">
+      <c r="S11" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="T11" s="100"/>
+      <c r="T11" s="101"/>
       <c r="U11" s="5"/>
       <c r="V11" s="7">
         <v>1</v>
@@ -44665,18 +44960,18 @@
         <v>23</v>
       </c>
       <c r="AB11" s="3"/>
-      <c r="AC11" s="101" t="s">
+      <c r="AC11" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="AD11" s="101"/>
+      <c r="AD11" s="102"/>
     </row>
     <row r="12" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="100"/>
+      <c r="D12" s="101"/>
       <c r="E12" s="5"/>
       <c r="F12" s="7">
         <v>0</v>
@@ -44695,18 +44990,18 @@
         <v>23</v>
       </c>
       <c r="L12" s="3"/>
-      <c r="M12" s="101">
+      <c r="M12" s="102">
         <v>6</v>
       </c>
-      <c r="N12" s="101"/>
+      <c r="N12" s="102"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="100" t="s">
+      <c r="S12" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="T12" s="100"/>
+      <c r="T12" s="101"/>
       <c r="U12" s="5"/>
       <c r="V12" s="7">
         <v>1</v>
@@ -44725,18 +45020,18 @@
         <v>23</v>
       </c>
       <c r="AB12" s="3"/>
-      <c r="AC12" s="101" t="s">
+      <c r="AC12" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="AD12" s="101"/>
+      <c r="AD12" s="102"/>
     </row>
     <row r="13" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="100" t="s">
+      <c r="C13" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="100"/>
+      <c r="D13" s="101"/>
       <c r="E13" s="5"/>
       <c r="F13" s="7">
         <v>0</v>
@@ -44755,18 +45050,18 @@
         <v>23</v>
       </c>
       <c r="L13" s="3"/>
-      <c r="M13" s="101">
+      <c r="M13" s="102">
         <v>7</v>
       </c>
-      <c r="N13" s="101"/>
+      <c r="N13" s="102"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="100" t="s">
+      <c r="S13" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="T13" s="100"/>
+      <c r="T13" s="101"/>
       <c r="U13" s="5"/>
       <c r="V13" s="7">
         <v>1</v>
@@ -44785,10 +45080,10 @@
         <v>23</v>
       </c>
       <c r="AB13" s="3"/>
-      <c r="AC13" s="101" t="s">
+      <c r="AC13" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="AD13" s="101"/>
+      <c r="AD13" s="102"/>
     </row>
     <row r="14" spans="1:37" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -45008,43 +45303,43 @@
     <row r="21" spans="1:37" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
       <c r="B21" s="36"/>
-      <c r="C21" s="102" t="s">
+      <c r="C21" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="102"/>
+      <c r="D21" s="100"/>
       <c r="E21" s="37"/>
-      <c r="F21" s="102" t="s">
+      <c r="F21" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="102"/>
+      <c r="G21" s="100"/>
       <c r="H21" s="37"/>
       <c r="I21" s="37"/>
       <c r="J21" s="37"/>
-      <c r="K21" s="102" t="s">
+      <c r="K21" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="102"/>
-      <c r="M21" s="102"/>
-      <c r="N21" s="102"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
+      <c r="N21" s="100"/>
       <c r="O21" s="37"/>
       <c r="P21" s="37"/>
       <c r="Q21" s="37"/>
       <c r="R21" s="36"/>
-      <c r="S21" s="102" t="s">
+      <c r="S21" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="T21" s="102"/>
+      <c r="T21" s="100"/>
       <c r="U21" s="6"/>
-      <c r="V21" s="102" t="s">
+      <c r="V21" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="W21" s="102"/>
-      <c r="AA21" s="102" t="s">
+      <c r="W21" s="100"/>
+      <c r="AA21" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="AB21" s="102"/>
-      <c r="AC21" s="102"/>
-      <c r="AD21" s="102"/>
+      <c r="AB21" s="100"/>
+      <c r="AC21" s="100"/>
+      <c r="AD21" s="100"/>
     </row>
     <row r="22" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -45073,15 +45368,15 @@
     <row r="23" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="100" t="s">
+      <c r="C23" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="100"/>
+      <c r="D23" s="101"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="101">
+      <c r="F23" s="102">
         <v>0</v>
       </c>
-      <c r="G23" s="101"/>
+      <c r="G23" s="102"/>
       <c r="H23" s="3"/>
       <c r="I23" s="5" t="s">
         <v>23</v>
@@ -45103,15 +45398,15 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
-      <c r="S23" s="100" t="s">
+      <c r="S23" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="T23" s="100"/>
+      <c r="T23" s="101"/>
       <c r="U23" s="5"/>
-      <c r="V23" s="101">
+      <c r="V23" s="102">
         <v>8</v>
       </c>
-      <c r="W23" s="101"/>
+      <c r="W23" s="102"/>
       <c r="Y23" s="5" t="s">
         <v>23</v>
       </c>
@@ -45131,15 +45426,15 @@
     <row r="24" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="100"/>
+      <c r="D24" s="101"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="101">
+      <c r="F24" s="102">
         <v>1</v>
       </c>
-      <c r="G24" s="101"/>
+      <c r="G24" s="102"/>
       <c r="H24" s="3"/>
       <c r="I24" s="5" t="s">
         <v>23</v>
@@ -45161,15 +45456,15 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
-      <c r="S24" s="100" t="s">
+      <c r="S24" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="T24" s="100"/>
+      <c r="T24" s="101"/>
       <c r="U24" s="5"/>
-      <c r="V24" s="101">
+      <c r="V24" s="102">
         <v>9</v>
       </c>
-      <c r="W24" s="101"/>
+      <c r="W24" s="102"/>
       <c r="Y24" s="5" t="s">
         <v>23</v>
       </c>
@@ -45189,15 +45484,15 @@
     <row r="25" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="100"/>
+      <c r="D25" s="101"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="101">
+      <c r="F25" s="102">
         <v>2</v>
       </c>
-      <c r="G25" s="101"/>
+      <c r="G25" s="102"/>
       <c r="H25" s="3"/>
       <c r="I25" s="5" t="s">
         <v>23</v>
@@ -45219,15 +45514,15 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="100">
+      <c r="S25" s="101">
         <v>10</v>
       </c>
-      <c r="T25" s="100"/>
+      <c r="T25" s="101"/>
       <c r="U25" s="5"/>
-      <c r="V25" s="101" t="s">
+      <c r="V25" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="W25" s="101"/>
+      <c r="W25" s="102"/>
       <c r="Y25" s="5" t="s">
         <v>23</v>
       </c>
@@ -45247,15 +45542,15 @@
     <row r="26" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="100" t="s">
+      <c r="C26" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="100"/>
+      <c r="D26" s="101"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="101">
+      <c r="F26" s="102">
         <v>3</v>
       </c>
-      <c r="G26" s="101"/>
+      <c r="G26" s="102"/>
       <c r="H26" s="3"/>
       <c r="I26" s="5" t="s">
         <v>23</v>
@@ -45277,15 +45572,15 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
-      <c r="S26" s="100" t="s">
+      <c r="S26" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="T26" s="100"/>
+      <c r="T26" s="101"/>
       <c r="U26" s="5"/>
-      <c r="V26" s="101" t="s">
+      <c r="V26" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="W26" s="101"/>
+      <c r="W26" s="102"/>
       <c r="Y26" s="5" t="s">
         <v>23</v>
       </c>
@@ -45305,15 +45600,15 @@
     <row r="27" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="100" t="s">
+      <c r="C27" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="100"/>
+      <c r="D27" s="101"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="101">
+      <c r="F27" s="102">
         <v>4</v>
       </c>
-      <c r="G27" s="101"/>
+      <c r="G27" s="102"/>
       <c r="H27" s="3"/>
       <c r="I27" s="5" t="s">
         <v>23</v>
@@ -45335,15 +45630,15 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="100" t="s">
+      <c r="S27" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="T27" s="100"/>
+      <c r="T27" s="101"/>
       <c r="U27" s="5"/>
-      <c r="V27" s="101" t="s">
+      <c r="V27" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="W27" s="101"/>
+      <c r="W27" s="102"/>
       <c r="Y27" s="5" t="s">
         <v>23</v>
       </c>
@@ -45363,15 +45658,15 @@
     <row r="28" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="100" t="s">
+      <c r="C28" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="100"/>
+      <c r="D28" s="101"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="101">
+      <c r="F28" s="102">
         <v>5</v>
       </c>
-      <c r="G28" s="101"/>
+      <c r="G28" s="102"/>
       <c r="H28" s="3"/>
       <c r="I28" s="5" t="s">
         <v>23</v>
@@ -45393,15 +45688,15 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="100" t="s">
+      <c r="S28" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="T28" s="100"/>
+      <c r="T28" s="101"/>
       <c r="U28" s="5"/>
-      <c r="V28" s="101" t="s">
+      <c r="V28" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="W28" s="101"/>
+      <c r="W28" s="102"/>
       <c r="Y28" s="5" t="s">
         <v>23</v>
       </c>
@@ -45421,15 +45716,15 @@
     <row r="29" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="100" t="s">
+      <c r="C29" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="100"/>
+      <c r="D29" s="101"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="101">
+      <c r="F29" s="102">
         <v>6</v>
       </c>
-      <c r="G29" s="101"/>
+      <c r="G29" s="102"/>
       <c r="H29" s="3"/>
       <c r="I29" s="5" t="s">
         <v>23</v>
@@ -45451,15 +45746,15 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="100" t="s">
+      <c r="S29" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="T29" s="100"/>
+      <c r="T29" s="101"/>
       <c r="U29" s="5"/>
-      <c r="V29" s="101" t="s">
+      <c r="V29" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="W29" s="101"/>
+      <c r="W29" s="102"/>
       <c r="Y29" s="5" t="s">
         <v>23</v>
       </c>
@@ -45479,15 +45774,15 @@
     <row r="30" spans="1:37" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="100"/>
+      <c r="D30" s="101"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="101">
+      <c r="F30" s="102">
         <v>7</v>
       </c>
-      <c r="G30" s="101"/>
+      <c r="G30" s="102"/>
       <c r="H30" s="3"/>
       <c r="I30" s="5" t="s">
         <v>23</v>
@@ -45509,15 +45804,15 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="100" t="s">
+      <c r="S30" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="T30" s="100"/>
+      <c r="T30" s="101"/>
       <c r="U30" s="5"/>
-      <c r="V30" s="101" t="s">
+      <c r="V30" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="W30" s="101"/>
+      <c r="W30" s="102"/>
       <c r="Y30" s="5" t="s">
         <v>23</v>
       </c>
@@ -45536,36 +45831,38 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="AA21:AD21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="V25:W25"/>
     <mergeCell ref="A1:AK1"/>
     <mergeCell ref="A18:AK18"/>
     <mergeCell ref="S21:T21"/>
@@ -45582,38 +45879,36 @@
     <mergeCell ref="S10:T10"/>
     <mergeCell ref="AC10:AD10"/>
     <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="AA21:AD21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>